<commit_message>
saved volcano fig as png
</commit_message>
<xml_diff>
--- a/src/group_4/original_test_data.xlsx
+++ b/src/group_4/original_test_data.xlsx
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.1653681309792389</v>
+        <v>-0.05124647226819731</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9982631631469887</v>
+        <v>0.1165340111754933</v>
       </c>
     </row>
     <row r="3">
@@ -481,10 +481,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.1304776031658144</v>
+        <v>1.075908433645916</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2707065775094799</v>
+        <v>0.2562821896478944</v>
       </c>
     </row>
     <row r="4">
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.206856327632903</v>
+        <v>-0.862585156419838</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9511291738229287</v>
+        <v>0.6123848634545964</v>
       </c>
     </row>
     <row r="5">
@@ -512,8 +512,12 @@
           <t>Gene3</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>-0.5915662200416927</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.5692498516767089</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -525,10 +529,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>-1.200917297060415</v>
+        <v>0.496115412931781</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2813172160874803</v>
+        <v>0.9776611205750612</v>
       </c>
     </row>
     <row r="7">
@@ -541,10 +545,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.5776762239163629</v>
+        <v>0.8059997732670778</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3785363920709374</v>
+        <v>0.08373810287694738</v>
       </c>
     </row>
     <row r="8">
@@ -557,10 +561,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6187824947632695</v>
+        <v>-0.960430868263573</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6719485790017069</v>
+        <v>0.05704740441803435</v>
       </c>
     </row>
     <row r="9">
@@ -573,10 +577,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1.467032065966825</v>
+        <v>-1.283276340877165</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9061371980589886</v>
+        <v>0.3729204079113255</v>
       </c>
     </row>
     <row r="10">
@@ -589,10 +593,10 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-1.18082582613209</v>
+        <v>-1.910412512405695</v>
       </c>
       <c r="D10" t="n">
-        <v>0.2894598625520097</v>
+        <v>0.5160798982943893</v>
       </c>
     </row>
     <row r="11">
@@ -605,10 +609,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.2481411644160024</v>
+        <v>-0.07993869337389428</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9671589041522273</v>
+        <v>0.5065168976828339</v>
       </c>
     </row>
     <row r="12">
@@ -621,10 +625,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1.089000525511098</v>
+        <v>-0.9222513109305691</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8924245242796348</v>
+        <v>0.2090149122343908</v>
       </c>
     </row>
     <row r="13">
@@ -637,10 +641,10 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.7635701033121185</v>
+        <v>-0.8010957157747601</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3201111890201366</v>
+        <v>0.6147907800365555</v>
       </c>
     </row>
     <row r="14">
@@ -653,10 +657,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.6920598300099373</v>
+        <v>1.591884368780668</v>
       </c>
       <c r="D14" t="n">
-        <v>0.628492796254471</v>
+        <v>0.06501636056340265</v>
       </c>
     </row>
     <row r="15">
@@ -669,10 +673,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.4706206287263505</v>
+        <v>-0.3210274743165798</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6042073462622254</v>
+        <v>0.19669365233223</v>
       </c>
     </row>
     <row r="16">
@@ -684,8 +688,12 @@
           <t>Gene14</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+      <c r="C16" t="n">
+        <v>0.7173680415153602</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.06267052133251527</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -697,10 +705,10 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.9246771118063308</v>
+        <v>0.7245411693416838</v>
       </c>
       <c r="D17" t="n">
-        <v>0.08220904367597792</v>
+        <v>0.1190185795011929</v>
       </c>
     </row>
     <row r="18">
@@ -713,10 +721,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1.07291033449456</v>
+        <v>-1.655342758868531</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2597285056624802</v>
+        <v>0.1228246884167578</v>
       </c>
     </row>
     <row r="19">
@@ -729,10 +737,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.5327785257096734</v>
+        <v>-0.3226804151994406</v>
       </c>
       <c r="D19" t="n">
-        <v>0.2935936632621688</v>
+        <v>0.6615440383159179</v>
       </c>
     </row>
     <row r="20">
@@ -744,8 +752,12 @@
           <t>Gene18</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>-0.2911080528624239</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.9841847084960202</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -757,10 +769,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.2432227680117011</v>
+        <v>-1.530124231068745</v>
       </c>
       <c r="D21" t="n">
-        <v>0.9522805898641654</v>
+        <v>0.6643174011264494</v>
       </c>
     </row>
     <row r="22">
@@ -773,10 +785,10 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>-0.2511680161801246</v>
+        <v>0.8804113352684855</v>
       </c>
       <c r="D22" t="n">
-        <v>0.3457689647525946</v>
+        <v>0.5943418104231554</v>
       </c>
     </row>
     <row r="23">
@@ -789,10 +801,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1.006973958174987</v>
+        <v>-1.631203511293053</v>
       </c>
       <c r="D23" t="n">
-        <v>0.6138220694715329</v>
+        <v>0.04702208276932096</v>
       </c>
     </row>
     <row r="24">
@@ -805,10 +817,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-1.164854306879456</v>
+        <v>0.1664752793604172</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6960267755056569</v>
+        <v>0.03769099897736761</v>
       </c>
     </row>
     <row r="25">
@@ -820,12 +832,8 @@
           <t>Gene23</t>
         </is>
       </c>
-      <c r="C25" t="n">
-        <v>0.5601956753459505</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.3359083950143058</v>
-      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -837,10 +845,10 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.05846293347803515</v>
+        <v>0.1524179177153441</v>
       </c>
       <c r="D26" t="n">
-        <v>0.9856797835485256</v>
+        <v>0.02689275956014825</v>
       </c>
     </row>
     <row r="27">
@@ -853,10 +861,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.5544637799607255</v>
+        <v>1.845735829739362</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4690754475451673</v>
+        <v>0.1024339862552363</v>
       </c>
     </row>
     <row r="28">
@@ -868,12 +876,8 @@
           <t>Gene26</t>
         </is>
       </c>
-      <c r="C28" t="n">
-        <v>-0.469119260344623</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.2498500108725339</v>
-      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -885,10 +889,10 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1.310349825199663</v>
+        <v>-0.3759048248361666</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5957985164118361</v>
+        <v>0.5243939033757079</v>
       </c>
     </row>
     <row r="30">
@@ -901,10 +905,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.6896013826876192</v>
+        <v>1.611479909065487</v>
       </c>
       <c r="D30" t="n">
-        <v>0.6655273218017721</v>
+        <v>0.6586129274711541</v>
       </c>
     </row>
     <row r="31">
@@ -917,10 +921,10 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.4167854242241124</v>
+        <v>-0.4397314157413</v>
       </c>
       <c r="D31" t="n">
-        <v>0.604520107791689</v>
+        <v>0.01672104550168652</v>
       </c>
     </row>
     <row r="32">
@@ -933,10 +937,10 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.4729025501347344</v>
+        <v>-1.402825564917863</v>
       </c>
       <c r="D32" t="n">
-        <v>0.9837603192284057</v>
+        <v>0.7075175117503557</v>
       </c>
     </row>
     <row r="33">
@@ -949,10 +953,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.7289599970906465</v>
+        <v>0.2210867955338335</v>
       </c>
       <c r="D33" t="n">
-        <v>0.6014738313419248</v>
+        <v>0.9696923261399181</v>
       </c>
     </row>
     <row r="34">
@@ -965,10 +969,10 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1.75314660343455</v>
+        <v>-0.7420197696734002</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9110126994150441</v>
+        <v>0.4619784935688916</v>
       </c>
     </row>
     <row r="35">
@@ -981,10 +985,10 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.7475848859371745</v>
+        <v>-0.2750984841495288</v>
       </c>
       <c r="D35" t="n">
-        <v>0.9655998186865919</v>
+        <v>0.6487584902811252</v>
       </c>
     </row>
     <row r="36">
@@ -1009,10 +1013,10 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.6191321205738315</v>
+        <v>0.5603937532529546</v>
       </c>
       <c r="D37" t="n">
-        <v>0.163618191932974</v>
+        <v>0.8307877469683947</v>
       </c>
     </row>
     <row r="38">
@@ -1025,10 +1029,10 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>-0.1478107754665143</v>
+        <v>-0.8242859282563622</v>
       </c>
       <c r="D38" t="n">
-        <v>0.5478364554366643</v>
+        <v>0.9581095100560945</v>
       </c>
     </row>
     <row r="39">
@@ -1041,10 +1045,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>-0.2190888810859746</v>
+        <v>2.444120456206064</v>
       </c>
       <c r="D39" t="n">
-        <v>0.6555786559922134</v>
+        <v>0.04638484900854045</v>
       </c>
     </row>
     <row r="40">
@@ -1057,10 +1061,10 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.9977076772857931</v>
+        <v>0.7686132473480797</v>
       </c>
       <c r="D40" t="n">
-        <v>0.3478058605916916</v>
+        <v>0.5562684433367024</v>
       </c>
     </row>
     <row r="41">
@@ -1073,10 +1077,10 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.4624542946715045</v>
+        <v>1.374239120819454</v>
       </c>
       <c r="D41" t="n">
-        <v>0.9590482377061821</v>
+        <v>0.5349678785378849</v>
       </c>
     </row>
     <row r="42">
@@ -1089,10 +1093,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>-0.2593452175059062</v>
+        <v>0.6350520075353919</v>
       </c>
       <c r="D42" t="n">
-        <v>0.1635854197877763</v>
+        <v>0.8006116038739939</v>
       </c>
     </row>
     <row r="43">
@@ -1105,10 +1109,10 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.8306583691353462</v>
+        <v>-0.5915642819854271</v>
       </c>
       <c r="D43" t="n">
-        <v>0.9577097104871646</v>
+        <v>0.7411920224712418</v>
       </c>
     </row>
     <row r="44">
@@ -1121,10 +1125,10 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>-0.1880655871386492</v>
+        <v>0.2704931499780999</v>
       </c>
       <c r="D44" t="n">
-        <v>0.5793180506209729</v>
+        <v>0.8253233326976952</v>
       </c>
     </row>
     <row r="45">
@@ -1137,10 +1141,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>-0.1619874948261688</v>
+        <v>-0.4462513212349941</v>
       </c>
       <c r="D45" t="n">
-        <v>0.3023475772212445</v>
+        <v>0.2720473610571977</v>
       </c>
     </row>
     <row r="46">
@@ -1153,10 +1157,10 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>-0.388625249073256</v>
+        <v>-0.2381837668807433</v>
       </c>
       <c r="D46" t="n">
-        <v>0.2770759320392679</v>
+        <v>0.01342513702925496</v>
       </c>
     </row>
     <row r="47">
@@ -1169,10 +1173,10 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.5470466355745963</v>
+        <v>-1.111909800864932</v>
       </c>
       <c r="D47" t="n">
-        <v>0.7344538928139444</v>
+        <v>0.02363084715052655</v>
       </c>
     </row>
     <row r="48">
@@ -1184,8 +1188,12 @@
           <t>Gene46</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+      <c r="C48" t="n">
+        <v>0.9775695303819989</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.07164632373198765</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -1196,8 +1204,12 @@
           <t>Gene47</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
+      <c r="C49" t="n">
+        <v>-0.3850449240827401</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.9190747315660529</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -1209,10 +1221,10 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>-1.290975215266389</v>
+        <v>1.02066401306132</v>
       </c>
       <c r="D50" t="n">
-        <v>0.6213709471940485</v>
+        <v>0.550157945931504</v>
       </c>
     </row>
     <row r="51">
@@ -1225,10 +1237,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>-1.377711026186198</v>
+        <v>-0.4285865435911622</v>
       </c>
       <c r="D51" t="n">
-        <v>0.1291530150693327</v>
+        <v>0.9896147455832123</v>
       </c>
     </row>
     <row r="52">
@@ -1240,8 +1252,12 @@
           <t>Gene50</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr"/>
+      <c r="C52" t="n">
+        <v>-0.3463420192076028</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.6433319544610455</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1253,10 +1269,10 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>-1.831260995164885</v>
+        <v>-0.9223454756643625</v>
       </c>
       <c r="D53" t="n">
-        <v>0.06883019434530813</v>
+        <v>0.6445743966068982</v>
       </c>
     </row>
     <row r="54">
@@ -1268,12 +1284,8 @@
           <t>Gene52</t>
         </is>
       </c>
-      <c r="C54" t="n">
-        <v>0.6851807173302363</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0.2136920068623227</v>
-      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1285,10 +1297,10 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>0.5016004480919433</v>
+        <v>-0.1602341770834688</v>
       </c>
       <c r="D55" t="n">
-        <v>0.2464843674462839</v>
+        <v>0.2985668078690291</v>
       </c>
     </row>
     <row r="56">
@@ -1301,10 +1313,10 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>-0.1730331499021266</v>
+        <v>-0.6574329302513127</v>
       </c>
       <c r="D56" t="n">
-        <v>0.04505903918705334</v>
+        <v>0.344312488365936</v>
       </c>
     </row>
     <row r="57">
@@ -1317,10 +1329,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>-0.7581625058661928</v>
+        <v>-0.7706613668751215</v>
       </c>
       <c r="D57" t="n">
-        <v>0.8065957724360584</v>
+        <v>0.8915941815112437</v>
       </c>
     </row>
     <row r="58">
@@ -1333,10 +1345,10 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>-0.199787010832955</v>
+        <v>0.9145294978714179</v>
       </c>
       <c r="D58" t="n">
-        <v>0.6661171237065543</v>
+        <v>0.34396456277867</v>
       </c>
     </row>
     <row r="59">
@@ -1349,10 +1361,10 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.8575456992572401</v>
+        <v>0.1944381031280404</v>
       </c>
       <c r="D59" t="n">
-        <v>0.2421266753241617</v>
+        <v>0.3699989987543775</v>
       </c>
     </row>
     <row r="60">
@@ -1365,10 +1377,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>-0.3466662002257431</v>
+        <v>1.430469462501794</v>
       </c>
       <c r="D60" t="n">
-        <v>0.7273232773864081</v>
+        <v>0.6088044527644301</v>
       </c>
     </row>
     <row r="61">
@@ -1381,10 +1393,10 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>-0.3762558011174523</v>
+        <v>-1.574250373019882</v>
       </c>
       <c r="D61" t="n">
-        <v>0.426475918125367</v>
+        <v>0.865040112261611</v>
       </c>
     </row>
     <row r="62">
@@ -1397,10 +1409,10 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.007998638351679438</v>
+        <v>-0.9636819929880518</v>
       </c>
       <c r="D62" t="n">
-        <v>0.7236259482129265</v>
+        <v>0.3424253452754747</v>
       </c>
     </row>
     <row r="63">
@@ -1413,10 +1425,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>-0.3210111013584009</v>
+        <v>-0.1053520452352895</v>
       </c>
       <c r="D63" t="n">
-        <v>0.4570818223502175</v>
+        <v>0.9645360165064154</v>
       </c>
     </row>
     <row r="64">
@@ -1429,10 +1441,10 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.3341913461622376</v>
+        <v>0.001385285828498836</v>
       </c>
       <c r="D64" t="n">
-        <v>0.4051311598379063</v>
+        <v>0.6365474652221111</v>
       </c>
     </row>
     <row r="65">
@@ -1444,12 +1456,8 @@
           <t>Gene63</t>
         </is>
       </c>
-      <c r="C65" t="n">
-        <v>0.4222113157217916</v>
-      </c>
-      <c r="D65" t="n">
-        <v>0.09318480365963167</v>
-      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1461,10 +1469,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1.373263240921624</v>
+        <v>0.8289027458449272</v>
       </c>
       <c r="D66" t="n">
-        <v>0.9953056797096334</v>
+        <v>0.8419375912535541</v>
       </c>
     </row>
     <row r="67">
@@ -1477,10 +1485,10 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.4101481889415384</v>
+        <v>-0.3566807741546517</v>
       </c>
       <c r="D67" t="n">
-        <v>0.9503552037934451</v>
+        <v>0.2131188243232254</v>
       </c>
     </row>
     <row r="68">
@@ -1493,10 +1501,10 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>-0.02781670141032837</v>
+        <v>-1.896545956671251</v>
       </c>
       <c r="D68" t="n">
-        <v>0.7169743916065181</v>
+        <v>0.9746195414982775</v>
       </c>
     </row>
     <row r="69">
@@ -1509,10 +1517,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.648743368379131</v>
+        <v>-0.05818895410316782</v>
       </c>
       <c r="D69" t="n">
-        <v>0.6158582677772548</v>
+        <v>0.6423275673554977</v>
       </c>
     </row>
     <row r="70">
@@ -1525,10 +1533,10 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>-0.3916986650681559</v>
+        <v>-1.754990556949109</v>
       </c>
       <c r="D70" t="n">
-        <v>0.01833150112623461</v>
+        <v>0.002724282840635417</v>
       </c>
     </row>
     <row r="71">
@@ -1541,10 +1549,10 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>-1.57133297652146</v>
+        <v>0.4033832801608584</v>
       </c>
       <c r="D71" t="n">
-        <v>0.6343635549236207</v>
+        <v>0.5441148321379273</v>
       </c>
     </row>
     <row r="72">
@@ -1556,8 +1564,12 @@
           <t>Gene70</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
+      <c r="C72" t="n">
+        <v>0.2088812391504386</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.5753301617450718</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -1569,10 +1581,10 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>-0.002637003188734809</v>
+        <v>1.4396483170419</v>
       </c>
       <c r="D73" t="n">
-        <v>0.3574819895091789</v>
+        <v>0.3138981979377987</v>
       </c>
     </row>
     <row r="74">
@@ -1585,10 +1597,10 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>-0.8746477457166012</v>
+        <v>-1.599052686908847</v>
       </c>
       <c r="D74" t="n">
-        <v>0.5427470913819441</v>
+        <v>0.1968248684760824</v>
       </c>
     </row>
     <row r="75">
@@ -1600,12 +1612,8 @@
           <t>Gene73</t>
         </is>
       </c>
-      <c r="C75" t="n">
-        <v>-0.7544528163905427</v>
-      </c>
-      <c r="D75" t="n">
-        <v>0.4141215627964357</v>
-      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -1616,8 +1624,12 @@
           <t>Gene74</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
+      <c r="C76" t="n">
+        <v>1.556366527463733</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.5858971137754244</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -1629,10 +1641,10 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>-0.3548331446273981</v>
+        <v>0.09205738119948087</v>
       </c>
       <c r="D77" t="n">
-        <v>0.2283793873777096</v>
+        <v>0.03099507291631654</v>
       </c>
     </row>
     <row r="78">
@@ -1645,10 +1657,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.3020258276330735</v>
+        <v>-0.1405579790414384</v>
       </c>
       <c r="D78" t="n">
-        <v>0.9642195172392026</v>
+        <v>0.0709138775051058</v>
       </c>
     </row>
     <row r="79">
@@ -1661,10 +1673,10 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1.240081655216082</v>
+        <v>-0.541458759951653</v>
       </c>
       <c r="D79" t="n">
-        <v>0.4174830644825008</v>
+        <v>0.5588197190438194</v>
       </c>
     </row>
     <row r="80">
@@ -1677,10 +1689,10 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1.38684697691646</v>
+        <v>-0.4386298772198119</v>
       </c>
       <c r="D80" t="n">
-        <v>0.3940474662807673</v>
+        <v>0.339486897531738</v>
       </c>
     </row>
     <row r="81">
@@ -1692,12 +1704,8 @@
           <t>Gene79</t>
         </is>
       </c>
-      <c r="C81" t="n">
-        <v>-1.145194877091071</v>
-      </c>
-      <c r="D81" t="n">
-        <v>0.746607619022517</v>
-      </c>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -1709,10 +1717,10 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>-1.194043597000688</v>
+        <v>-1.770940778519035</v>
       </c>
       <c r="D82" t="n">
-        <v>0.446579519493548</v>
+        <v>0.2627873695400764</v>
       </c>
     </row>
     <row r="83">
@@ -1725,10 +1733,10 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.4140860367422072</v>
+        <v>-0.5930212646339734</v>
       </c>
       <c r="D83" t="n">
-        <v>0.9020474223770991</v>
+        <v>0.8136768373783398</v>
       </c>
     </row>
     <row r="84">
@@ -1740,8 +1748,12 @@
           <t>Gene82</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr"/>
+      <c r="C84" t="n">
+        <v>-1.359318862453168</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.8206599874585043</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -1753,10 +1765,10 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.1859757940631192</v>
+        <v>0.5542485346813597</v>
       </c>
       <c r="D85" t="n">
-        <v>0.7732982746016154</v>
+        <v>0.3550442399372543</v>
       </c>
     </row>
     <row r="86">
@@ -1769,10 +1781,10 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>-0.3579862353301719</v>
+        <v>-1.329515986631947</v>
       </c>
       <c r="D86" t="n">
-        <v>0.6174656153496033</v>
+        <v>0.5997861353974804</v>
       </c>
     </row>
     <row r="87">
@@ -1785,10 +1797,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.2088500951234241</v>
+        <v>0.3181974179141019</v>
       </c>
       <c r="D87" t="n">
-        <v>0.7735136834346299</v>
+        <v>0.2987334853664169</v>
       </c>
     </row>
     <row r="88">
@@ -1801,10 +1813,10 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1.190630939524693</v>
+        <v>-2.514551893717444</v>
       </c>
       <c r="D88" t="n">
-        <v>0.2467480460924211</v>
+        <v>0.8960125092786448</v>
       </c>
     </row>
     <row r="89">
@@ -1817,10 +1829,10 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>-0.694455192844579</v>
+        <v>-2.137024664737153</v>
       </c>
       <c r="D89" t="n">
-        <v>0.330962147064782</v>
+        <v>0.2618206529954723</v>
       </c>
     </row>
     <row r="90">
@@ -1833,10 +1845,10 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>-0.3776926100130155</v>
+        <v>1.769882961555094</v>
       </c>
       <c r="D90" t="n">
-        <v>0.08671067279878575</v>
+        <v>0.2279298648862725</v>
       </c>
     </row>
     <row r="91">
@@ -1849,10 +1861,10 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>-0.2545307726150272</v>
+        <v>2.3629718871612</v>
       </c>
       <c r="D91" t="n">
-        <v>0.643891512634297</v>
+        <v>0.3658031577842265</v>
       </c>
     </row>
     <row r="92">
@@ -1865,10 +1877,10 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.06687303725151104</v>
+        <v>0.1599691707801534</v>
       </c>
       <c r="D92" t="n">
-        <v>0.691366316568196</v>
+        <v>0.6220653903370444</v>
       </c>
     </row>
     <row r="93">
@@ -1881,10 +1893,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0.6331382142396962</v>
+        <v>-0.7485677948369388</v>
       </c>
       <c r="D93" t="n">
-        <v>0.3093980063565711</v>
+        <v>0.8852216133753907</v>
       </c>
     </row>
     <row r="94">
@@ -1896,12 +1908,8 @@
           <t>Gene92</t>
         </is>
       </c>
-      <c r="C94" t="n">
-        <v>-0.6747741239653152</v>
-      </c>
-      <c r="D94" t="n">
-        <v>0.8116371060475009</v>
-      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -1913,10 +1921,10 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.3113916213495354</v>
+        <v>-1.398782842501166</v>
       </c>
       <c r="D95" t="n">
-        <v>0.2784264412815771</v>
+        <v>0.9878382817221761</v>
       </c>
     </row>
     <row r="96">
@@ -1929,10 +1937,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.5053939167786086</v>
+        <v>1.226975111151378</v>
       </c>
       <c r="D96" t="n">
-        <v>0.7048905648438533</v>
+        <v>0.5022998301901366</v>
       </c>
     </row>
     <row r="97">
@@ -1944,12 +1952,8 @@
           <t>Gene95</t>
         </is>
       </c>
-      <c r="C97" t="n">
-        <v>-0.5154451309342122</v>
-      </c>
-      <c r="D97" t="n">
-        <v>0.603392397378765</v>
-      </c>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -1961,10 +1965,10 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>-0.03838543319655365</v>
+        <v>0.172941246157735</v>
       </c>
       <c r="D98" t="n">
-        <v>0.9152306291724237</v>
+        <v>0.1673830032250285</v>
       </c>
     </row>
     <row r="99">
@@ -1976,12 +1980,8 @@
           <t>Gene97</t>
         </is>
       </c>
-      <c r="C99" t="n">
-        <v>0.5858289620253245</v>
-      </c>
-      <c r="D99" t="n">
-        <v>0.6573947960579462</v>
-      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -1993,10 +1993,10 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>-0.5389039620704624</v>
+        <v>1.415584947771703</v>
       </c>
       <c r="D100" t="n">
-        <v>0.66273774239711</v>
+        <v>0.9726268232037465</v>
       </c>
     </row>
     <row r="101">
@@ -2009,10 +2009,10 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>-0.07706225805857254</v>
+        <v>-1.479720995396407</v>
       </c>
       <c r="D101" t="n">
-        <v>0.9538757150224482</v>
+        <v>0.3922692406903486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>